<commit_message>
sua password de loi
</commit_message>
<xml_diff>
--- a/Equivalence.xlsx
+++ b/Equivalence.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hoang Luu\OneDrive - ctnprox\Documents\RegisterTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A4F5AFD-B047-43DB-BC7B-1FD3EF8B393A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F718041-C1CF-4F39-8F62-CE6711EA4F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CD6C0BB-F102-4652-8F5E-4972E5710F4C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CD6C0BB-F102-4652-8F5E-4972E5710F4C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>Mật khẩu ít nhất 6 kí tự</t>
   </si>
@@ -83,40 +84,173 @@
     <t>Case</t>
   </si>
   <si>
-    <t>"Đăng ký thành công"</t>
-  </si>
-  <si>
-    <t>"Tên không được để trông"</t>
-  </si>
-  <si>
-    <t>"Tên có có kí tự đặc biệt hoặc số"</t>
-  </si>
-  <si>
-    <t>"Email để trống"</t>
-  </si>
-  <si>
-    <t>"Mật khẩu ít nhất 6 kí tự"</t>
-  </si>
-  <si>
-    <t>"Email đã tồn tại"</t>
-  </si>
-  <si>
-    <t>"Mật khẩu không hợp lệ"</t>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Nhập lại mật khẩu giống với mật khẩu đã nhập</t>
+  </si>
+  <si>
+    <t>Nhập lại mật khẩu không giống với mật khẩu đã nhập</t>
+  </si>
+  <si>
+    <t>SUCCESS-Hiển thị "Đăng ký thành công"</t>
+  </si>
+  <si>
+    <t>FAIL-Hiển thị "Tên không được để trông"</t>
+  </si>
+  <si>
+    <t>FAIL-Hiển thị "Tên có có kí tự đặc biệt hoặc số"</t>
+  </si>
+  <si>
+    <t>FAIL-Hiển thị "Email để trống"</t>
+  </si>
+  <si>
+    <t>FAIL-Hiển thị "Email đã tồn tại"</t>
+  </si>
+  <si>
+    <t>FAIL-Hiển thị "Mật khẩu không hợp lệ"</t>
+  </si>
+  <si>
+    <t>FAIL-Hiển thị "Mật khẩu nhập lại không khớp"</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>re-password</t>
+  </si>
+  <si>
+    <t>dgadyuasgyui</t>
+  </si>
+  <si>
+    <t>dyagygs@gmail.com</t>
+  </si>
+  <si>
+    <t>Aa123456@</t>
+  </si>
+  <si>
+    <t>dyagyfgs@gmail.com</t>
+  </si>
+  <si>
+    <t>dgsdsgf032#$#</t>
+  </si>
+  <si>
+    <t>d2agygs@gmail.com</t>
+  </si>
+  <si>
+    <t>gvdavsgvsa</t>
+  </si>
+  <si>
+    <t>adsadasd</t>
+  </si>
+  <si>
+    <t>dyagy685s@gmail.com</t>
+  </si>
+  <si>
+    <t>Aa6@</t>
+  </si>
+  <si>
+    <t>dyag23ygs@gmail.com</t>
+  </si>
+  <si>
+    <t>Aabcdefgh@</t>
+  </si>
+  <si>
+    <t>dyagy0gs@gmail.com</t>
+  </si>
+  <si>
+    <t>Aabcdefg0</t>
+  </si>
+  <si>
+    <t>dyagy9gs@gmail.com</t>
+  </si>
+  <si>
+    <t>abcdefgh@</t>
+  </si>
+  <si>
+    <t>dyagy9fgs@gmail.com</t>
+  </si>
+  <si>
+    <t>abcdefgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kết quả </t>
+  </si>
+  <si>
+    <t>Lý giải</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Dev chưa kiểm tra email đã tồn tại</t>
+  </si>
+  <si>
+    <t>Dev chưa kiểm tra độ dài mật khẩu</t>
+  </si>
+  <si>
+    <t>Dev chưa kiểm tra mật khẩu phải có số</t>
+  </si>
+  <si>
+    <t>Dev chưa kiểm tra mật khẩu phải có ký tự đặc biệt</t>
+  </si>
+  <si>
+    <t>Dev chưa kiểm tra mật khẩu phải có ký tự in hoa</t>
+  </si>
+  <si>
+    <t>Dev chưa kiểm tra mật khẩu nhập lại phải trùng khớp với mật khẩu đã nhập</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,12 +259,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -151,19 +309,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -211,30 +356,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,261 +709,623 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9536B6D7-B066-46DF-A733-6BA7B2272CE2}">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94EA1DB9-9408-4AC4-9C73-490621B5B1A9}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="19.625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="14.75" customWidth="1"/>
+    <col min="5" max="5" width="9.875" customWidth="1"/>
+    <col min="7" max="7" width="20.375" style="21" customWidth="1"/>
+    <col min="8" max="8" width="34.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A85ED6B3-A19D-4809-B979-1CE19BD9982C}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{D84AE3D1-FD8C-473B-9FDF-F20172FE1E68}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{9219C24C-7EC5-47B9-9B6B-06C3C9DA5AF3}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{CD08462D-6271-4EB0-8E10-CDAC568AFA1D}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{4FC46B5E-0CFF-4AB3-9FA0-F4F5838E3A29}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{08EB95BA-9B90-481C-8861-B7A6E9C13C86}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{A654F55C-DE07-4A96-8B00-3B058E23F3D8}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{90AAD1F4-3696-40B8-A0F4-82C7BF6972DF}"/>
+    <hyperlink ref="C7" r:id="rId9" xr:uid="{77C73173-AFF7-4DF0-AFC6-3E4456E0BE63}"/>
+    <hyperlink ref="B8:B10" r:id="rId10" display="dyagygs@gmail.com" xr:uid="{8638B985-009D-4ECD-8FC7-F6F39E7C7F25}"/>
+    <hyperlink ref="C8" r:id="rId11" xr:uid="{7B15AB8C-522A-4ECC-A7EC-8465A485DE01}"/>
+    <hyperlink ref="C9:C10" r:id="rId12" display="Aabcdefgh@" xr:uid="{E7D4D7FE-4252-4E34-8D7D-929833207256}"/>
+    <hyperlink ref="C10" r:id="rId13" xr:uid="{BAA3FF04-CB08-4BC4-8AE3-FFC3D9A4B27C}"/>
+    <hyperlink ref="B4" r:id="rId14" xr:uid="{6FBCA20D-60D9-44DE-BFB6-29B3AE54D042}"/>
+    <hyperlink ref="C4" r:id="rId15" xr:uid="{F48D0C80-198F-4DDF-B4E6-FC53B446F8A7}"/>
+    <hyperlink ref="B8" r:id="rId16" xr:uid="{F3C1D64F-A204-4288-BB81-3804F2FE2B0A}"/>
+    <hyperlink ref="B10" r:id="rId17" xr:uid="{BDA72147-2868-42AD-A33C-095759DDB65B}"/>
+    <hyperlink ref="B9" r:id="rId18" xr:uid="{D8AC2C51-67D5-48A2-A1E4-00B1112B133C}"/>
+    <hyperlink ref="D2" r:id="rId19" xr:uid="{2C702621-EE08-47A0-90EC-D7484C78A02C}"/>
+    <hyperlink ref="D3:D6" r:id="rId20" display="Aa123456@" xr:uid="{169719D1-2632-4D00-B89D-B0FEBCDF9A40}"/>
+    <hyperlink ref="D7" r:id="rId21" xr:uid="{63C00450-4BA2-4A7D-B9EB-80B029C29F15}"/>
+    <hyperlink ref="D8" r:id="rId22" xr:uid="{52A48AD1-6F1C-4EF9-8F36-86FAF4E5CCF2}"/>
+    <hyperlink ref="D9:D10" r:id="rId23" display="Aabcdefgh@" xr:uid="{4738614A-368B-4E4D-A228-56D75370AC8D}"/>
+    <hyperlink ref="D10" r:id="rId24" xr:uid="{A9107DF0-931F-4BB8-B44B-43EDE64887B0}"/>
+    <hyperlink ref="B11" r:id="rId25" xr:uid="{6FF47B3B-FC77-4A75-9132-631528B8B24C}"/>
+    <hyperlink ref="C11" r:id="rId26" xr:uid="{A6D44C5E-7188-426F-86BB-F7A58C42F771}"/>
+    <hyperlink ref="D11" r:id="rId27" display="abcdefgh@" xr:uid="{CA5CD113-EDAD-4F05-AC99-1E40ADCC90C4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9536B6D7-B066-46DF-A733-6BA7B2272CE2}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48" customWidth="1"/>
-    <col min="3" max="3" width="33.625" customWidth="1"/>
-    <col min="9" max="9" width="31.25" customWidth="1"/>
+    <col min="2" max="2" width="7.25" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
+    <col min="4" max="4" width="7.25" customWidth="1"/>
+    <col min="10" max="10" width="43.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="1" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="9">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2">
         <v>4</v>
       </c>
-      <c r="F2" s="1">
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9">
+        <v>6</v>
+      </c>
+      <c r="F3" s="10">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2">
+        <v>4</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>7</v>
+      </c>
+      <c r="F4" s="10">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2">
+        <v>4</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="9">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G5" s="10">
+        <v>7</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3</v>
+      </c>
+      <c r="I5" s="2">
+        <v>4</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10">
+        <v>8</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
+      <c r="I6" s="2">
+        <v>4</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H7" s="10">
+        <v>9</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="9">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="10">
+        <v>10</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="9">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="10">
+        <v>11</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8">
+        <v>4</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="9">
+        <v>13</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2</v>
+      </c>
+      <c r="H10" s="10">
+        <v>12</v>
+      </c>
+      <c r="I10" s="2">
+        <v>4</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
         <v>3</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1">
-        <v>4</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1">
-        <v>3</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="7">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1">
-        <v>5</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2</v>
-      </c>
-      <c r="H4" s="1">
-        <v>3</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
-        <v>3</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1">
-        <v>7</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>3</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1">
-        <v>8</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>2</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1">
-        <v>9</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="1">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1">
-        <v>2</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="F10" s="1">
-        <v>11</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
-        <v>2</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="I11" s="10">
+        <v>13</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="F1:H1"/>
+  <mergeCells count="1">
+    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100338B04ADEEB16F479B18FE20295EA3A2" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d830cdc3126ebdef5e2b4e1b6fb48812">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="654383a2-f530-41ff-8fce-3021cb9ef43b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f98c915c9a171d00ef13ec7db004128f" ns3:_="">
     <xsd:import namespace="654383a2-f530-41ff-8fce-3021cb9ef43b"/>
@@ -984,22 +1509,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4BD0468-557F-44B6-8343-B5795DD440C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C9EBE57-1D56-4BC3-B721-C4A0D6D729DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="654383a2-f530-41ff-8fce-3021cb9ef43b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{701F5707-3D41-4421-8FD5-4521125335A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1015,28 +1549,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4BD0468-557F-44B6-8343-B5795DD440C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C9EBE57-1D56-4BC3-B721-C4A0D6D729DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="654383a2-f530-41ff-8fce-3021cb9ef43b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>